<commit_message>
open cases about txn engine
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreecases/batchsql/sql_batchsql_cases_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreecases/batchsql/sql_batchsql_cases_btree.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
   <si>
     <t>TestID</t>
   </si>
@@ -446,6 +446,26 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/btreecases/batchsql/expectedresult/btree_batch_015.csv</t>
+  </si>
+  <si>
+    <t>btree_batch_016</t>
+  </si>
+  <si>
+    <t>批量操作语句16执行</t>
+  </si>
+  <si>
+    <t>btree_batch_sql_016</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/btreecases/batchsql/expectedresult/btree_batch_016.csv</t>
+  </si>
+  <si>
+    <t>select a.NAME as N from b as a order by a.ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -818,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -834,7 +854,7 @@
     <col min="6" max="6" width="8.5" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="21.625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="40.25" style="6" customWidth="1"/>
     <col min="11" max="11" width="17.5" style="6" customWidth="1"/>
     <col min="12" max="12" width="21.625" style="2" customWidth="1"/>
@@ -1377,6 +1397,38 @@
       </c>
       <c r="N16" s="6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>